<commit_message>
Role management with PIM and new acrobat reader deployment process
</commit_message>
<xml_diff>
--- a/data/aad/Lizenzen.xlsx
+++ b/data/aad/Lizenzen.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="493" documentId="11_7FBCCD06A469FE4EF57D3C6CA5C393DAEEC5EA02" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{95D90D06-469E-49FC-AAAC-26A787B71C5F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC258D27-C803-43DF-84ED-C05C8E45199D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2226" yWindow="420" windowWidth="15654" windowHeight="10902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lizenzübersicht" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lizenzübersicht!$A$5:$F$6</definedName>
   </definedNames>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -90,9 +93,6 @@
     <t>SPP1</t>
   </si>
   <si>
-    <t>MS365BUSBASIC</t>
-  </si>
-  <si>
     <t>VIRTPHONE</t>
   </si>
   <si>
@@ -103,6 +103,87 @@
   </si>
   <si>
     <t>first.last@alyaconsulting.ch</t>
+  </si>
+  <si>
+    <t>AADBASIC</t>
+  </si>
+  <si>
+    <t>AADP2</t>
+  </si>
+  <si>
+    <t>COMMPHONE</t>
+  </si>
+  <si>
+    <t>DYN365P1</t>
+  </si>
+  <si>
+    <t>EMS</t>
+  </si>
+  <si>
+    <t>EXCHP1</t>
+  </si>
+  <si>
+    <t>INTUNE</t>
+  </si>
+  <si>
+    <t>MS365BUSBASICFULL</t>
+  </si>
+  <si>
+    <t>MS365BUSSTDFULL</t>
+  </si>
+  <si>
+    <t>MS365E5FULL</t>
+  </si>
+  <si>
+    <t>O365E1FULL</t>
+  </si>
+  <si>
+    <t>O365E3FULL</t>
+  </si>
+  <si>
+    <t>PBIPRO</t>
+  </si>
+  <si>
+    <t>VISIO2</t>
+  </si>
+  <si>
+    <t>VIVATOP</t>
+  </si>
+  <si>
+    <t>Lic11</t>
+  </si>
+  <si>
+    <t>Lic12</t>
+  </si>
+  <si>
+    <t>Lic13</t>
+  </si>
+  <si>
+    <t>Lic14</t>
+  </si>
+  <si>
+    <t>Lic15</t>
+  </si>
+  <si>
+    <t>Lic16</t>
+  </si>
+  <si>
+    <t>Lic17</t>
+  </si>
+  <si>
+    <t>Lic18</t>
+  </si>
+  <si>
+    <t>Lic19</t>
+  </si>
+  <si>
+    <t>Lic20</t>
+  </si>
+  <si>
+    <t>Lic21</t>
+  </si>
+  <si>
+    <t>Lic22</t>
   </si>
 </sst>
 </file>
@@ -187,7 +268,21 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -241,6 +336,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Gruppen"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,7 +672,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
@@ -576,12 +684,11 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="37.1015625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="12.578125" style="2" customWidth="1"/>
-    <col min="7" max="11" width="12.578125" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="8.83984375" style="3"/>
+    <col min="2" max="23" width="15.05078125" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="8.83984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,13 +717,49 @@
         <v>17</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>23</v>
+      <c r="L1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -650,8 +793,44 @@
       <c r="K2" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -685,25 +864,61 @@
       <c r="K3" s="2">
         <v>1</v>
       </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+      <c r="S3" s="2">
+        <v>1</v>
+      </c>
+      <c r="T3" s="2">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1</v>
+      </c>
+      <c r="V3" s="2">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <f>SUBTOTAL(9,B6:B6)</f>
+        <f>SUBTOTAL(9,B6:B100)</f>
         <v>1</v>
       </c>
       <c r="C4" s="2">
-        <f>SUBTOTAL(9,C6:C6)</f>
+        <f>SUBTOTAL(9,C6:C100)</f>
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <f>SUBTOTAL(9,D6:D6)</f>
+        <f t="shared" ref="D4:W4" si="0">SUBTOTAL(9,D6:D100)</f>
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:J4" si="0">SUBTOTAL(9,E6:E6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4" s="2">
@@ -727,42 +942,132 @@
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4" si="1">SUBTOTAL(9,K6:K6)</f>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="N5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="U5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>21</v>
+      <c r="V5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -773,37 +1078,37 @@
       <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F6">
     <sortCondition ref="A6"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A4:C4 L4:XFD4 E4 G4 I4">
-    <cfRule type="expression" dxfId="5" priority="19" stopIfTrue="1">
+  <conditionalFormatting sqref="A4:XFD4">
+    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
       <formula>IF(A$4&gt;0,A$4&gt;A$3,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="20">
+    <cfRule type="expression" dxfId="6" priority="22">
       <formula>IF(A$4&gt;0,A$4&gt;(A$3-2),FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4 F4 H4 J4">
-    <cfRule type="expression" dxfId="3" priority="13" stopIfTrue="1">
-      <formula>IF(D$4&gt;0,D$4&gt;D$3,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="14">
-      <formula>IF(D$4&gt;0,D$4&gt;(D$3-2),FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>IF(K$4&gt;0,K$4&gt;K$3,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>IF(K$4&gt;0,K$4&gt;(K$3-2),FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -812,21 +1117,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -1010,10 +1300,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1366AA07-09C2-4356-9758-1591C4908924}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{916A2060-2461-4699-A876-3B8D996083A0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1035,19 +1350,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{916A2060-2461-4699-A876-3B8D996083A0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1366AA07-09C2-4356-9758-1591C4908924}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="353a1f37-f986-455b-adc7-292fbd315350"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
New groups for AD and licenses
</commit_message>
<xml_diff>
--- a/data/aad/Lizenzen.xlsx
+++ b/data/aad/Lizenzen.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D608128-55F6-4D45-9B4E-42C8BDA3F3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1D5A2A-306E-41EE-98C4-98128AD61B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="600" windowWidth="20652" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lizenzübersicht" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lizenzübersicht!$A$5:$I$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lizenzübersicht!$A$5:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>Lic25</t>
+  </si>
+  <si>
+    <t>Do not use,</t>
+  </si>
+  <si>
+    <t>assign to bundle</t>
+  </si>
+  <si>
+    <t>Lic26</t>
+  </si>
+  <si>
+    <t>EXCHARCHIVE</t>
   </si>
 </sst>
 </file>
@@ -289,21 +301,7 @@
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -680,7 +678,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
@@ -694,15 +692,15 @@
     <col min="1" max="1" width="37.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="2" customWidth="1"/>
     <col min="3" max="3" width="15" style="10" customWidth="1"/>
-    <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15" style="10" customWidth="1"/>
-    <col min="6" max="15" width="15" style="2" customWidth="1"/>
-    <col min="16" max="16" width="15" style="10" customWidth="1"/>
-    <col min="17" max="26" width="15" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.88671875" style="3"/>
+    <col min="4" max="13" width="15" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15" style="10" customWidth="1"/>
+    <col min="15" max="25" width="15" style="2" customWidth="1"/>
+    <col min="26" max="26" width="15" style="10" customWidth="1"/>
+    <col min="27" max="27" width="15" style="2" customWidth="1"/>
+    <col min="28" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,13 +713,13 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -733,13 +731,13 @@
       <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -751,13 +749,13 @@
       <c r="P1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="2" t="s">
         <v>46</v>
       </c>
       <c r="T1" s="2" t="s">
@@ -769,20 +767,23 @@
       <c r="V1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="2" t="s">
         <v>54</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA1" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -795,7 +796,7 @@
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -822,13 +823,13 @@
       <c r="M2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -858,11 +859,14 @@
       <c r="Y2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -875,7 +879,7 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2">
@@ -902,13 +906,13 @@
       <c r="M3" s="2">
         <v>1</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="10">
         <v>1</v>
       </c>
       <c r="O3" s="2">
         <v>1</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="2">
@@ -938,11 +942,14 @@
       <c r="Y3" s="2">
         <v>1</v>
       </c>
-      <c r="Z3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -958,29 +965,29 @@
         <f>SUBTOTAL(9,D6:D100)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="10">
-        <f>SUBTOTAL(9,E6:E97)</f>
+      <c r="E4" s="2">
+        <f>SUBTOTAL(9,E6:E100)</f>
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" ref="F4:Z4" si="0">SUBTOTAL(9,F6:F100)</f>
+        <f t="shared" ref="F4:X4" si="0">SUBTOTAL(9,F6:F100)</f>
         <v>0</v>
       </c>
       <c r="G4" s="2">
-        <f>SUBTOTAL(9,G6:G100)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
@@ -994,16 +1001,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N4" s="2">
-        <f t="shared" si="0"/>
+      <c r="N4" s="10">
+        <f>SUBTOTAL(9,N6:N97)</f>
         <v>0</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P4" s="10">
-        <f>SUBTOTAL(9,P6:P97)</f>
+      <c r="P4" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q4" s="2">
@@ -1039,15 +1046,17 @@
         <v>0</v>
       </c>
       <c r="Y4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Y4" si="1">SUBTOTAL(9,Y6:Y100)</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA4" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1060,74 +1069,77 @@
       <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="AA5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
@@ -1136,22 +1148,22 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7">
-        <v>1</v>
-      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="N6" s="10"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="10"/>
+      <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -1161,127 +1173,120 @@
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="7"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C7" s="10" t="str">
-        <f t="shared" ref="C7:C20" si="1">IF(OR(A7=1,B7=1),1,"")</f>
+        <f t="shared" ref="C7:C20" si="2">IF(OR(A7=1,B7=1),1,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C8" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C9" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C10" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C11" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C12" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C13" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C14" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C15" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C16" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:I6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:G6">
     <sortCondition ref="A6"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A4:B4 D4 F4:O4 Q4:XFD4">
-    <cfRule type="expression" dxfId="7" priority="27" stopIfTrue="1">
+  <conditionalFormatting sqref="A4:B4 D4:M4 O4:XFD4">
+    <cfRule type="expression" dxfId="5" priority="27" stopIfTrue="1">
       <formula>IF(A$4&gt;0,A$4&gt;A$3,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="28">
+    <cfRule type="expression" dxfId="4" priority="28">
       <formula>IF(A$4&gt;0,A$4&gt;(A$3-2),FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>IF(C$4&gt;0,C$4&gt;C$3,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>IF(C$4&gt;0,C$4&gt;(C$3-2),FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>IF(E$4&gt;0,E$4&gt;E$3,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>IF(E$4&gt;0,E$4&gt;(E$3-2),FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4">
+  <conditionalFormatting sqref="N4">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>IF(P$4&gt;0,P$4&gt;P$3,FALSE)</formula>
+      <formula>IF(N$4&gt;0,N$4&gt;N$3,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>IF(P$4&gt;0,P$4&gt;(P$3-2),FALSE)</formula>
+      <formula>IF(N$4&gt;0,N$4&gt;(N$3-2),FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1290,15 +1295,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBA446ED503E744880217BF491FB0C7B" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="27f6ebb53777ae95e550442d3878210b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="353a1f37-f986-455b-adc7-292fbd315350" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71df197f0939a0ed9a29c200b6a3be36" ns2:_="">
     <xsd:import namespace="353a1f37-f986-455b-adc7-292fbd315350"/>
@@ -1482,6 +1478,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1489,14 +1494,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1366AA07-09C2-4356-9758-1591C4908924}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{916A2060-2461-4699-A876-3B8D996083A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1510,6 +1507,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1366AA07-09C2-4356-9758-1591C4908924}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>